<commit_message>
checkbox functions implemented (110, 112)
</commit_message>
<xml_diff>
--- a/ExcelReaderScript/Testcase_1_date.xlsx
+++ b/ExcelReaderScript/Testcase_1_date.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
   <si>
     <t>Testcase name</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>[Phone]</t>
+  </si>
+  <si>
+    <t>testbench</t>
+  </si>
+  <si>
+    <t>SYS-110.tbc</t>
+  </si>
+  <si>
+    <t>SYS-112.tbc</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K1" sqref="K1:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,9 +504,10 @@
     <col min="8" max="8" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,8 +538,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -560,8 +573,11 @@
       <c r="J2" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -592,8 +608,11 @@
       <c r="J3" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -624,8 +643,11 @@
       <c r="J4" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -656,8 +678,11 @@
       <c r="J5" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -688,8 +713,11 @@
       <c r="J6" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -720,8 +748,11 @@
       <c r="J7" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -752,8 +783,11 @@
       <c r="J8" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -784,8 +818,11 @@
       <c r="J9" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -816,8 +853,11 @@
       <c r="J10" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -848,8 +888,11 @@
       <c r="J11" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -880,8 +923,11 @@
       <c r="J12" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -912,8 +958,11 @@
       <c r="J13" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -944,8 +993,11 @@
       <c r="J14" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -976,8 +1028,11 @@
       <c r="J15" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1008,8 +1063,11 @@
       <c r="J16" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -1037,8 +1095,11 @@
       <c r="J17" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1066,8 +1127,11 @@
       <c r="J18" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1094,6 +1158,9 @@
       </c>
       <c r="J19" s="5">
         <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>